<commit_message>
added data for notebooks
</commit_message>
<xml_diff>
--- a/DATA/presidents.xlsx
+++ b/DATA/presidents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jstrick/curr/courses/python/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8D0E75-27F6-7A4A-8B78-F7F3135D22AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89461B96-8258-E147-86C3-49B8A18847A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-64060" yWindow="-1140" windowWidth="28280" windowHeight="15920" tabRatio="988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US Presidents" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="283">
   <si>
     <t>Term</t>
   </si>
@@ -2767,17 +2767,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:C47"/>
+  <dimension ref="B2:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
@@ -3139,14 +3133,6 @@
         <v>277</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B47" t="s">
-        <v>280</v>
-      </c>
-      <c r="C47" t="s">
-        <v>281</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>